<commit_message>
actualizar marco con cambios def
</commit_message>
<xml_diff>
--- a/data/Marco acumulativo.xlsx
+++ b/data/Marco acumulativo.xlsx
@@ -1562,7 +1562,7 @@
         <v>14</v>
       </c>
       <c r="I39" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3464,7 +3464,7 @@
         <v>11</v>
       </c>
       <c r="E105" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F105" t="s">
         <v>11</v>
@@ -6631,7 +6631,7 @@
         <v>11</v>
       </c>
       <c r="G214" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H214" t="s">
         <v>14</v>
@@ -6848,22 +6848,22 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C222" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D222" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E222" t="s">
         <v>11</v>
       </c>
       <c r="F222" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G222" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H222" t="s">
         <v>12</v>
@@ -7176,7 +7176,7 @@
         <v>11</v>
       </c>
       <c r="E233" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F233" t="s">
         <v>11</v>
@@ -7591,7 +7591,7 @@
         <v>12</v>
       </c>
       <c r="H247" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I247" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
calificar estudiantes para pagina
</commit_message>
<xml_diff>
--- a/data/Marco acumulativo.xlsx
+++ b/data/Marco acumulativo.xlsx
@@ -55,9 +55,6 @@
     <t>1B</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>2A</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>2B</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>5</t>
@@ -477,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -486,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -503,10 +503,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -515,7 +515,7 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -532,11 +532,11 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -561,7 +561,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -573,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -593,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -602,7 +602,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -622,7 +622,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -631,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -660,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -680,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -689,7 +689,7 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -738,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -764,10 +764,10 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -793,10 +793,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -825,13 +825,13 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
@@ -866,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -877,13 +877,13 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -892,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -912,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -921,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
@@ -941,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -950,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
@@ -967,10 +967,10 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -979,7 +979,7 @@
         <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
@@ -999,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
@@ -1028,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -1037,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
@@ -1054,10 +1054,10 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1086,7 +1086,7 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -1095,7 +1095,7 @@
         <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
@@ -1115,7 +1115,7 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
@@ -1173,7 +1173,7 @@
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -1182,7 +1182,7 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
@@ -1202,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -1211,7 +1211,7 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I27" t="s">
         <v>12</v>
@@ -1231,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
@@ -1240,7 +1240,7 @@
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -1260,7 +1260,7 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
@@ -1289,7 +1289,7 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -1327,7 +1327,7 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
@@ -1347,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -1376,7 +1376,7 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1405,7 +1405,7 @@
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -1414,10 +1414,10 @@
         <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I34" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1431,10 +1431,10 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
@@ -1443,7 +1443,7 @@
         <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
@@ -1472,7 +1472,7 @@
         <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
@@ -1492,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -1501,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
@@ -1515,13 +1515,13 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -1544,13 +1544,13 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I39" t="s">
         <v>11</v>
@@ -1573,13 +1573,13 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -1588,10 +1588,10 @@
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1614,10 +1614,10 @@
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
@@ -1646,7 +1646,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I42" t="s">
         <v>11</v>
@@ -1666,7 +1666,7 @@
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -1675,7 +1675,7 @@
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I43" t="s">
         <v>11</v>
@@ -1704,10 +1704,10 @@
         <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1721,10 +1721,10 @@
         <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
         <v>11</v>
@@ -1733,7 +1733,7 @@
         <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I45" t="s">
         <v>12</v>
@@ -1750,10 +1750,10 @@
         <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -1762,7 +1762,7 @@
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I46" t="s">
         <v>11</v>
@@ -1791,10 +1791,10 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1811,7 +1811,7 @@
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -1820,7 +1820,7 @@
         <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I48" t="s">
         <v>11</v>
@@ -1840,7 +1840,7 @@
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -1849,7 +1849,7 @@
         <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I49" t="s">
         <v>11</v>
@@ -1869,7 +1869,7 @@
         <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
@@ -1907,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I51" t="s">
         <v>11</v>
@@ -1921,13 +1921,13 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52" t="s">
         <v>11</v>
@@ -1953,16 +1953,16 @@
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
         <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" t="s">
         <v>12</v>
@@ -1979,19 +1979,19 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F54" t="s">
         <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" t="s">
         <v>12</v>
@@ -2014,7 +2014,7 @@
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F55" t="s">
         <v>11</v>
@@ -2023,7 +2023,7 @@
         <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I55" t="s">
         <v>11</v>
@@ -2043,7 +2043,7 @@
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
         <v>11</v>
@@ -2052,7 +2052,7 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I56" t="s">
         <v>11</v>
@@ -2072,7 +2072,7 @@
         <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
@@ -2081,7 +2081,7 @@
         <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I57" t="s">
         <v>11</v>
@@ -2101,7 +2101,7 @@
         <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
         <v>11</v>
@@ -2110,7 +2110,7 @@
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I58" t="s">
         <v>11</v>
@@ -2130,7 +2130,7 @@
         <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
@@ -2139,7 +2139,7 @@
         <v>12</v>
       </c>
       <c r="H59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I59" t="s">
         <v>11</v>
@@ -2156,7 +2156,7 @@
         <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -2168,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I60" t="s">
         <v>11</v>
@@ -2188,7 +2188,7 @@
         <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F61" t="s">
         <v>11</v>
@@ -2197,7 +2197,7 @@
         <v>12</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I61" t="s">
         <v>11</v>
@@ -2217,7 +2217,7 @@
         <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F62" t="s">
         <v>11</v>
@@ -2226,7 +2226,7 @@
         <v>12</v>
       </c>
       <c r="H62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I62" t="s">
         <v>11</v>
@@ -2243,10 +2243,10 @@
         <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
         <v>12</v>
@@ -2255,7 +2255,7 @@
         <v>12</v>
       </c>
       <c r="H63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I63" t="s">
         <v>11</v>
@@ -2287,7 +2287,7 @@
         <v>12</v>
       </c>
       <c r="I64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2304,7 +2304,7 @@
         <v>11</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
         <v>11</v>
@@ -2313,7 +2313,7 @@
         <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I65" t="s">
         <v>11</v>
@@ -2362,7 +2362,7 @@
         <v>11</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F67" t="s">
         <v>11</v>
@@ -2388,7 +2388,7 @@
         <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -2420,7 +2420,7 @@
         <v>11</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
@@ -2429,7 +2429,7 @@
         <v>12</v>
       </c>
       <c r="H69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I69" t="s">
         <v>11</v>
@@ -2443,13 +2443,13 @@
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
         <v>11</v>
@@ -2472,11 +2472,11 @@
         <v>11</v>
       </c>
       <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
         <v>15</v>
       </c>
-      <c r="D71" t="s">
-        <v>16</v>
-      </c>
       <c r="E71" t="s">
         <v>12</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I71" t="s">
         <v>11</v>
@@ -2504,10 +2504,10 @@
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F72" t="s">
         <v>11</v>
@@ -2516,7 +2516,7 @@
         <v>12</v>
       </c>
       <c r="H72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I72" t="s">
         <v>11</v>
@@ -2536,7 +2536,7 @@
         <v>11</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
@@ -2545,7 +2545,7 @@
         <v>12</v>
       </c>
       <c r="H73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I73" t="s">
         <v>11</v>
@@ -2565,7 +2565,7 @@
         <v>11</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F74" t="s">
         <v>11</v>
@@ -2574,7 +2574,7 @@
         <v>12</v>
       </c>
       <c r="H74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I74" t="s">
         <v>11</v>
@@ -2594,7 +2594,7 @@
         <v>11</v>
       </c>
       <c r="E75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
@@ -2603,7 +2603,7 @@
         <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I75" t="s">
         <v>11</v>
@@ -2632,7 +2632,7 @@
         <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I76" t="s">
         <v>11</v>
@@ -2652,7 +2652,7 @@
         <v>11</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
@@ -2678,10 +2678,10 @@
         <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
@@ -2690,7 +2690,7 @@
         <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I78" t="s">
         <v>11</v>
@@ -2710,7 +2710,7 @@
         <v>11</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F79" t="s">
         <v>11</v>
@@ -2736,10 +2736,10 @@
         <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F80" t="s">
         <v>11</v>
@@ -2748,7 +2748,7 @@
         <v>12</v>
       </c>
       <c r="H80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I80" t="s">
         <v>12</v>
@@ -2768,7 +2768,7 @@
         <v>11</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F81" t="s">
         <v>11</v>
@@ -2780,7 +2780,7 @@
         <v>12</v>
       </c>
       <c r="I81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2806,10 +2806,10 @@
         <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2835,7 +2835,7 @@
         <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I83" t="s">
         <v>11</v>
@@ -2852,10 +2852,10 @@
         <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F84" t="s">
         <v>11</v>
@@ -2864,7 +2864,7 @@
         <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I84" t="s">
         <v>11</v>
@@ -2896,7 +2896,7 @@
         <v>11</v>
       </c>
       <c r="I85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -2913,7 +2913,7 @@
         <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F86" t="s">
         <v>11</v>
@@ -2922,10 +2922,10 @@
         <v>12</v>
       </c>
       <c r="H86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -2965,13 +2965,13 @@
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
@@ -2980,7 +2980,7 @@
         <v>12</v>
       </c>
       <c r="H88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I88" t="s">
         <v>11</v>
@@ -2994,13 +2994,13 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" t="s">
         <v>14</v>
-      </c>
-      <c r="D89" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" t="s">
-        <v>15</v>
       </c>
       <c r="F89" t="s">
         <v>11</v>
@@ -3029,7 +3029,7 @@
         <v>11</v>
       </c>
       <c r="E90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -3038,7 +3038,7 @@
         <v>12</v>
       </c>
       <c r="H90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I90" t="s">
         <v>12</v>
@@ -3081,10 +3081,10 @@
         <v>11</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E92" t="s">
         <v>12</v>
@@ -3116,7 +3116,7 @@
         <v>11</v>
       </c>
       <c r="E93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F93" t="s">
         <v>11</v>
@@ -3125,7 +3125,7 @@
         <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I93" t="s">
         <v>11</v>
@@ -3142,10 +3142,10 @@
         <v>12</v>
       </c>
       <c r="D94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F94" t="s">
         <v>11</v>
@@ -3154,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="H94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I94" t="s">
         <v>11</v>
@@ -3171,10 +3171,10 @@
         <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F95" t="s">
         <v>11</v>
@@ -3183,7 +3183,7 @@
         <v>12</v>
       </c>
       <c r="H95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I95" t="s">
         <v>12</v>
@@ -3212,7 +3212,7 @@
         <v>12</v>
       </c>
       <c r="H96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I96" t="s">
         <v>11</v>
@@ -3258,10 +3258,10 @@
         <v>12</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F98" t="s">
         <v>11</v>
@@ -3270,7 +3270,7 @@
         <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I98" t="s">
         <v>11</v>
@@ -3313,22 +3313,22 @@
         <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E100" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
       <c r="G100" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I100" t="s">
         <v>11</v>
@@ -3348,7 +3348,7 @@
         <v>11</v>
       </c>
       <c r="E101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F101" t="s">
         <v>11</v>
@@ -3374,10 +3374,10 @@
         <v>12</v>
       </c>
       <c r="D102" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E102" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F102" t="s">
         <v>11</v>
@@ -3400,13 +3400,13 @@
         <v>11</v>
       </c>
       <c r="C103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E103" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F103" t="s">
         <v>12</v>
@@ -3435,7 +3435,7 @@
         <v>11</v>
       </c>
       <c r="E104" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F104" t="s">
         <v>11</v>
@@ -3444,7 +3444,7 @@
         <v>12</v>
       </c>
       <c r="H104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I104" t="s">
         <v>11</v>
@@ -3458,13 +3458,13 @@
         <v>11</v>
       </c>
       <c r="C105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D105" t="s">
         <v>11</v>
       </c>
       <c r="E105" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F105" t="s">
         <v>11</v>
@@ -3473,7 +3473,7 @@
         <v>12</v>
       </c>
       <c r="H105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I105" t="s">
         <v>11</v>
@@ -3493,7 +3493,7 @@
         <v>11</v>
       </c>
       <c r="E106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F106" t="s">
         <v>11</v>
@@ -3516,7 +3516,7 @@
         <v>11</v>
       </c>
       <c r="C107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
@@ -3531,7 +3531,7 @@
         <v>12</v>
       </c>
       <c r="H107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I107" t="s">
         <v>11</v>
@@ -3551,7 +3551,7 @@
         <v>11</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F108" t="s">
         <v>11</v>
@@ -3560,7 +3560,7 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I108" t="s">
         <v>11</v>
@@ -3580,7 +3580,7 @@
         <v>11</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F109" t="s">
         <v>11</v>
@@ -3589,7 +3589,7 @@
         <v>12</v>
       </c>
       <c r="H109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I109" t="s">
         <v>11</v>
@@ -3609,7 +3609,7 @@
         <v>11</v>
       </c>
       <c r="E110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F110" t="s">
         <v>11</v>
@@ -3632,13 +3632,13 @@
         <v>11</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D111" t="s">
         <v>11</v>
       </c>
       <c r="E111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F111" t="s">
         <v>11</v>
@@ -3647,7 +3647,7 @@
         <v>12</v>
       </c>
       <c r="H111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I111" t="s">
         <v>11</v>
@@ -3664,10 +3664,10 @@
         <v>12</v>
       </c>
       <c r="D112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F112" t="s">
         <v>11</v>
@@ -3693,10 +3693,10 @@
         <v>12</v>
       </c>
       <c r="D113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F113" t="s">
         <v>11</v>
@@ -3705,7 +3705,7 @@
         <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I113" t="s">
         <v>11</v>
@@ -3725,7 +3725,7 @@
         <v>11</v>
       </c>
       <c r="E114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F114" t="s">
         <v>11</v>
@@ -3754,7 +3754,7 @@
         <v>11</v>
       </c>
       <c r="E115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F115" t="s">
         <v>11</v>
@@ -3763,7 +3763,7 @@
         <v>11</v>
       </c>
       <c r="H115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I115" t="s">
         <v>11</v>
@@ -3777,13 +3777,13 @@
         <v>11</v>
       </c>
       <c r="C116" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D116" t="s">
         <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F116" t="s">
         <v>11</v>
@@ -3792,7 +3792,7 @@
         <v>12</v>
       </c>
       <c r="H116" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I116" t="s">
         <v>11</v>
@@ -3806,13 +3806,13 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D117" t="s">
         <v>11</v>
       </c>
       <c r="E117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F117" t="s">
         <v>11</v>
@@ -3838,10 +3838,10 @@
         <v>12</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F118" t="s">
         <v>11</v>
@@ -3867,10 +3867,10 @@
         <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F119" t="s">
         <v>11</v>
@@ -3899,7 +3899,7 @@
         <v>11</v>
       </c>
       <c r="E120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F120" t="s">
         <v>11</v>
@@ -3925,10 +3925,10 @@
         <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F121" t="s">
         <v>11</v>
@@ -3937,7 +3937,7 @@
         <v>12</v>
       </c>
       <c r="H121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I121" t="s">
         <v>11</v>
@@ -3951,13 +3951,13 @@
         <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D122" t="s">
         <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F122" t="s">
         <v>11</v>
@@ -3966,10 +3966,10 @@
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -3983,10 +3983,10 @@
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F123" t="s">
         <v>11</v>
@@ -3995,7 +3995,7 @@
         <v>12</v>
       </c>
       <c r="H123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I123" t="s">
         <v>11</v>
@@ -4012,10 +4012,10 @@
         <v>12</v>
       </c>
       <c r="D124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E124" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F124" t="s">
         <v>11</v>
@@ -4024,7 +4024,7 @@
         <v>12</v>
       </c>
       <c r="H124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I124" t="s">
         <v>11</v>
@@ -4070,7 +4070,7 @@
         <v>12</v>
       </c>
       <c r="D126" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E126" t="s">
         <v>12</v>
@@ -4082,7 +4082,7 @@
         <v>12</v>
       </c>
       <c r="H126" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I126" t="s">
         <v>11</v>
@@ -4096,7 +4096,7 @@
         <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D127" t="s">
         <v>11</v>
@@ -4157,10 +4157,10 @@
         <v>12</v>
       </c>
       <c r="D129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F129" t="s">
         <v>11</v>
@@ -4212,13 +4212,13 @@
         <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D131" t="s">
         <v>11</v>
       </c>
       <c r="E131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F131" t="s">
         <v>11</v>
@@ -4227,7 +4227,7 @@
         <v>12</v>
       </c>
       <c r="H131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I131" t="s">
         <v>11</v>
@@ -4241,22 +4241,22 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D132" t="s">
         <v>11</v>
       </c>
       <c r="E132" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F132" t="s">
         <v>11</v>
       </c>
       <c r="G132" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I132" t="s">
         <v>11</v>
@@ -4285,7 +4285,7 @@
         <v>12</v>
       </c>
       <c r="H133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I133" t="s">
         <v>11</v>
@@ -4305,7 +4305,7 @@
         <v>11</v>
       </c>
       <c r="E134" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F134" t="s">
         <v>11</v>
@@ -4331,16 +4331,16 @@
         <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F135" t="s">
         <v>11</v>
       </c>
       <c r="G135" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H135" t="s">
         <v>11</v>
@@ -4363,7 +4363,7 @@
         <v>11</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F136" t="s">
         <v>11</v>
@@ -4421,7 +4421,7 @@
         <v>11</v>
       </c>
       <c r="E138" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F138" t="s">
         <v>11</v>
@@ -4430,7 +4430,7 @@
         <v>12</v>
       </c>
       <c r="H138" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I138" t="s">
         <v>11</v>
@@ -4444,13 +4444,13 @@
         <v>11</v>
       </c>
       <c r="C139" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D139" t="s">
         <v>11</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F139" t="s">
         <v>11</v>
@@ -4488,7 +4488,7 @@
         <v>12</v>
       </c>
       <c r="H140" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I140" t="s">
         <v>11</v>
@@ -4505,7 +4505,7 @@
         <v>12</v>
       </c>
       <c r="D141" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E141" t="s">
         <v>12</v>
@@ -4534,10 +4534,10 @@
         <v>12</v>
       </c>
       <c r="D142" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E142" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F142" t="s">
         <v>11</v>
@@ -4592,10 +4592,10 @@
         <v>12</v>
       </c>
       <c r="D144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F144" t="s">
         <v>11</v>
@@ -4624,7 +4624,7 @@
         <v>11</v>
       </c>
       <c r="E145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F145" t="s">
         <v>11</v>
@@ -4633,7 +4633,7 @@
         <v>11</v>
       </c>
       <c r="H145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I145" t="s">
         <v>11</v>
@@ -4653,7 +4653,7 @@
         <v>11</v>
       </c>
       <c r="E146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F146" t="s">
         <v>11</v>
@@ -4662,10 +4662,10 @@
         <v>12</v>
       </c>
       <c r="H146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -4679,10 +4679,10 @@
         <v>12</v>
       </c>
       <c r="D147" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E147" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F147" t="s">
         <v>11</v>
@@ -4734,16 +4734,16 @@
         <v>11</v>
       </c>
       <c r="C149" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" t="s">
         <v>15</v>
       </c>
-      <c r="D149" t="s">
-        <v>16</v>
-      </c>
       <c r="E149" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F149" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G149" t="s">
         <v>17</v>
@@ -4766,10 +4766,10 @@
         <v>12</v>
       </c>
       <c r="D150" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E150" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F150" t="s">
         <v>11</v>
@@ -4778,7 +4778,7 @@
         <v>11</v>
       </c>
       <c r="H150" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I150" t="s">
         <v>11</v>
@@ -4894,7 +4894,7 @@
         <v>12</v>
       </c>
       <c r="H154" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I154" t="s">
         <v>11</v>
@@ -4917,7 +4917,7 @@
         <v>12</v>
       </c>
       <c r="F155" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G155" t="s">
         <v>12</v>
@@ -4972,7 +4972,7 @@
         <v>11</v>
       </c>
       <c r="E157" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F157" t="s">
         <v>11</v>
@@ -4981,7 +4981,7 @@
         <v>12</v>
       </c>
       <c r="H157" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I157" t="s">
         <v>11</v>
@@ -4995,7 +4995,7 @@
         <v>11</v>
       </c>
       <c r="C158" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D158" t="s">
         <v>11</v>
@@ -5007,10 +5007,10 @@
         <v>11</v>
       </c>
       <c r="G158" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H158" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I158" t="s">
         <v>12</v>
@@ -5030,7 +5030,7 @@
         <v>11</v>
       </c>
       <c r="E159" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F159" t="s">
         <v>11</v>
@@ -5059,7 +5059,7 @@
         <v>11</v>
       </c>
       <c r="E160" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F160" t="s">
         <v>11</v>
@@ -5068,7 +5068,7 @@
         <v>12</v>
       </c>
       <c r="H160" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I160" t="s">
         <v>11</v>
@@ -5088,7 +5088,7 @@
         <v>11</v>
       </c>
       <c r="E161" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F161" t="s">
         <v>11</v>
@@ -5097,7 +5097,7 @@
         <v>12</v>
       </c>
       <c r="H161" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I161" t="s">
         <v>11</v>
@@ -5117,7 +5117,7 @@
         <v>11</v>
       </c>
       <c r="E162" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F162" t="s">
         <v>12</v>
@@ -5126,7 +5126,7 @@
         <v>12</v>
       </c>
       <c r="H162" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I162" t="s">
         <v>11</v>
@@ -5155,10 +5155,10 @@
         <v>12</v>
       </c>
       <c r="H163" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I163" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -5169,14 +5169,14 @@
         <v>11</v>
       </c>
       <c r="C164" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164" t="s">
         <v>14</v>
       </c>
-      <c r="D164" t="s">
-        <v>11</v>
-      </c>
-      <c r="E164" t="s">
-        <v>15</v>
-      </c>
       <c r="F164" t="s">
         <v>11</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>12</v>
       </c>
       <c r="H164" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I164" t="s">
         <v>11</v>
@@ -5198,16 +5198,16 @@
         <v>11</v>
       </c>
       <c r="C165" t="s">
+        <v>14</v>
+      </c>
+      <c r="D165" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" t="s">
         <v>15</v>
       </c>
-      <c r="D165" t="s">
-        <v>11</v>
-      </c>
-      <c r="E165" t="s">
-        <v>16</v>
-      </c>
       <c r="F165" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G165" t="s">
         <v>12</v>
@@ -5242,7 +5242,7 @@
         <v>12</v>
       </c>
       <c r="H166" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I166" t="s">
         <v>11</v>
@@ -5256,13 +5256,13 @@
         <v>11</v>
       </c>
       <c r="C167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
       </c>
       <c r="E167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F167" t="s">
         <v>11</v>
@@ -5271,7 +5271,7 @@
         <v>12</v>
       </c>
       <c r="H167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I167" t="s">
         <v>12</v>
@@ -5285,13 +5285,13 @@
         <v>11</v>
       </c>
       <c r="C168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F168" t="s">
         <v>11</v>
@@ -5300,7 +5300,7 @@
         <v>12</v>
       </c>
       <c r="H168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I168" t="s">
         <v>11</v>
@@ -5314,22 +5314,22 @@
         <v>11</v>
       </c>
       <c r="C169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G169" t="s">
         <v>12</v>
       </c>
       <c r="H169" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I169" t="s">
         <v>11</v>
@@ -5358,7 +5358,7 @@
         <v>12</v>
       </c>
       <c r="H170" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I170" t="s">
         <v>11</v>
@@ -5372,7 +5372,7 @@
         <v>11</v>
       </c>
       <c r="C171" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
@@ -5387,7 +5387,7 @@
         <v>12</v>
       </c>
       <c r="H171" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I171" t="s">
         <v>11</v>
@@ -5407,7 +5407,7 @@
         <v>11</v>
       </c>
       <c r="E172" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F172" t="s">
         <v>11</v>
@@ -5416,7 +5416,7 @@
         <v>12</v>
       </c>
       <c r="H172" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I172" t="s">
         <v>11</v>
@@ -5445,7 +5445,7 @@
         <v>12</v>
       </c>
       <c r="H173" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I173" t="s">
         <v>11</v>
@@ -5485,22 +5485,22 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C175" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D175" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E175" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F175" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G175" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H175" t="s">
         <v>12</v>
@@ -5520,7 +5520,7 @@
         <v>12</v>
       </c>
       <c r="D176" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E176" t="s">
         <v>12</v>
@@ -5532,7 +5532,7 @@
         <v>12</v>
       </c>
       <c r="H176" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I176" t="s">
         <v>11</v>
@@ -5552,7 +5552,7 @@
         <v>11</v>
       </c>
       <c r="E177" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F177" t="s">
         <v>11</v>
@@ -5581,7 +5581,7 @@
         <v>11</v>
       </c>
       <c r="E178" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F178" t="s">
         <v>11</v>
@@ -5590,7 +5590,7 @@
         <v>12</v>
       </c>
       <c r="H178" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I178" t="s">
         <v>11</v>
@@ -5610,7 +5610,7 @@
         <v>11</v>
       </c>
       <c r="E179" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F179" t="s">
         <v>11</v>
@@ -5639,7 +5639,7 @@
         <v>11</v>
       </c>
       <c r="E180" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F180" t="s">
         <v>11</v>
@@ -5648,7 +5648,7 @@
         <v>12</v>
       </c>
       <c r="H180" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I180" t="s">
         <v>11</v>
@@ -5677,7 +5677,7 @@
         <v>12</v>
       </c>
       <c r="H181" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I181" t="s">
         <v>11</v>
@@ -5694,10 +5694,10 @@
         <v>12</v>
       </c>
       <c r="D182" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E182" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F182" t="s">
         <v>11</v>
@@ -5706,7 +5706,7 @@
         <v>12</v>
       </c>
       <c r="H182" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I182" t="s">
         <v>11</v>
@@ -5723,10 +5723,10 @@
         <v>12</v>
       </c>
       <c r="D183" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E183" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F183" t="s">
         <v>11</v>
@@ -5735,7 +5735,7 @@
         <v>12</v>
       </c>
       <c r="H183" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I183" t="s">
         <v>11</v>
@@ -5755,16 +5755,16 @@
         <v>11</v>
       </c>
       <c r="E184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F184" t="s">
         <v>11</v>
       </c>
       <c r="G184" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I184" t="s">
         <v>11</v>
@@ -5784,7 +5784,7 @@
         <v>11</v>
       </c>
       <c r="E185" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F185" t="s">
         <v>11</v>
@@ -5793,7 +5793,7 @@
         <v>12</v>
       </c>
       <c r="H185" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I185" t="s">
         <v>11</v>
@@ -5848,10 +5848,10 @@
         <v>11</v>
       </c>
       <c r="G187" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H187" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I187" t="s">
         <v>11</v>
@@ -5865,13 +5865,13 @@
         <v>11</v>
       </c>
       <c r="C188" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D188" t="s">
         <v>11</v>
       </c>
       <c r="E188" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F188" t="s">
         <v>11</v>
@@ -5880,7 +5880,7 @@
         <v>12</v>
       </c>
       <c r="H188" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I188" t="s">
         <v>11</v>
@@ -5894,13 +5894,13 @@
         <v>11</v>
       </c>
       <c r="C189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D189" t="s">
         <v>11</v>
       </c>
       <c r="E189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F189" t="s">
         <v>11</v>
@@ -5909,7 +5909,7 @@
         <v>12</v>
       </c>
       <c r="H189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I189" t="s">
         <v>11</v>
@@ -5955,10 +5955,10 @@
         <v>12</v>
       </c>
       <c r="D191" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E191" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F191" t="s">
         <v>11</v>
@@ -5967,7 +5967,7 @@
         <v>12</v>
       </c>
       <c r="H191" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I191" t="s">
         <v>11</v>
@@ -5984,10 +5984,10 @@
         <v>12</v>
       </c>
       <c r="D192" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E192" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F192" t="s">
         <v>11</v>
@@ -6010,13 +6010,13 @@
         <v>11</v>
       </c>
       <c r="C193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F193" t="s">
         <v>11</v>
@@ -6025,7 +6025,7 @@
         <v>12</v>
       </c>
       <c r="H193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I193" t="s">
         <v>11</v>
@@ -6039,7 +6039,7 @@
         <v>11</v>
       </c>
       <c r="C194" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -6074,7 +6074,7 @@
         <v>11</v>
       </c>
       <c r="E195" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F195" t="s">
         <v>11</v>
@@ -6100,19 +6100,19 @@
         <v>12</v>
       </c>
       <c r="D196" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E196" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F196" t="s">
         <v>11</v>
       </c>
       <c r="G196" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H196" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I196" t="s">
         <v>11</v>
@@ -6129,10 +6129,10 @@
         <v>12</v>
       </c>
       <c r="D197" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E197" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F197" t="s">
         <v>11</v>
@@ -6141,7 +6141,7 @@
         <v>12</v>
       </c>
       <c r="H197" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I197" t="s">
         <v>11</v>
@@ -6158,10 +6158,10 @@
         <v>12</v>
       </c>
       <c r="D198" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E198" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F198" t="s">
         <v>11</v>
@@ -6170,7 +6170,7 @@
         <v>12</v>
       </c>
       <c r="H198" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I198" t="s">
         <v>11</v>
@@ -6199,7 +6199,7 @@
         <v>12</v>
       </c>
       <c r="H199" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I199" t="s">
         <v>11</v>
@@ -6248,7 +6248,7 @@
         <v>11</v>
       </c>
       <c r="E201" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F201" t="s">
         <v>11</v>
@@ -6274,10 +6274,10 @@
         <v>12</v>
       </c>
       <c r="D202" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E202" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F202" t="s">
         <v>11</v>
@@ -6286,7 +6286,7 @@
         <v>12</v>
       </c>
       <c r="H202" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I202" t="s">
         <v>12</v>
@@ -6318,7 +6318,7 @@
         <v>12</v>
       </c>
       <c r="I203" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -6347,7 +6347,7 @@
         <v>12</v>
       </c>
       <c r="I204" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -6361,10 +6361,10 @@
         <v>12</v>
       </c>
       <c r="D205" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E205" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F205" t="s">
         <v>11</v>
@@ -6373,7 +6373,7 @@
         <v>12</v>
       </c>
       <c r="H205" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I205" t="s">
         <v>11</v>
@@ -6390,10 +6390,10 @@
         <v>12</v>
       </c>
       <c r="D206" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E206" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F206" t="s">
         <v>11</v>
@@ -6402,7 +6402,7 @@
         <v>11</v>
       </c>
       <c r="H206" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I206" t="s">
         <v>11</v>
@@ -6477,10 +6477,10 @@
         <v>12</v>
       </c>
       <c r="D209" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E209" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F209" t="s">
         <v>11</v>
@@ -6489,7 +6489,7 @@
         <v>12</v>
       </c>
       <c r="H209" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I209" t="s">
         <v>11</v>
@@ -6503,13 +6503,13 @@
         <v>11</v>
       </c>
       <c r="C210" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
       </c>
       <c r="E210" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F210" t="s">
         <v>11</v>
@@ -6538,7 +6538,7 @@
         <v>11</v>
       </c>
       <c r="E211" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F211" t="s">
         <v>11</v>
@@ -6547,7 +6547,7 @@
         <v>12</v>
       </c>
       <c r="H211" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I211" t="s">
         <v>11</v>
@@ -6576,7 +6576,7 @@
         <v>12</v>
       </c>
       <c r="H212" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I212" t="s">
         <v>11</v>
@@ -6593,7 +6593,7 @@
         <v>12</v>
       </c>
       <c r="D213" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E213" t="s">
         <v>12</v>
@@ -6622,7 +6622,7 @@
         <v>12</v>
       </c>
       <c r="D214" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E214" t="s">
         <v>12</v>
@@ -6634,7 +6634,7 @@
         <v>12</v>
       </c>
       <c r="H214" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I214" t="s">
         <v>11</v>
@@ -6651,10 +6651,10 @@
         <v>12</v>
       </c>
       <c r="D215" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E215" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F215" t="s">
         <v>11</v>
@@ -6683,7 +6683,7 @@
         <v>11</v>
       </c>
       <c r="E216" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F216" t="s">
         <v>11</v>
@@ -6712,7 +6712,7 @@
         <v>11</v>
       </c>
       <c r="E217" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F217" t="s">
         <v>11</v>
@@ -6721,7 +6721,7 @@
         <v>12</v>
       </c>
       <c r="H217" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I217" t="s">
         <v>11</v>
@@ -6750,7 +6750,7 @@
         <v>12</v>
       </c>
       <c r="H218" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I218" t="s">
         <v>11</v>
@@ -6767,10 +6767,10 @@
         <v>12</v>
       </c>
       <c r="D219" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E219" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F219" t="s">
         <v>11</v>
@@ -6779,7 +6779,7 @@
         <v>12</v>
       </c>
       <c r="H219" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I219" t="s">
         <v>11</v>
@@ -6796,10 +6796,10 @@
         <v>12</v>
       </c>
       <c r="D220" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E220" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F220" t="s">
         <v>11</v>
@@ -6808,7 +6808,7 @@
         <v>12</v>
       </c>
       <c r="H220" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I220" t="s">
         <v>11</v>
@@ -6837,7 +6837,7 @@
         <v>12</v>
       </c>
       <c r="H221" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I221" t="s">
         <v>11</v>
@@ -6880,13 +6880,13 @@
         <v>11</v>
       </c>
       <c r="C223" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E223" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F223" t="s">
         <v>12</v>
@@ -6895,7 +6895,7 @@
         <v>12</v>
       </c>
       <c r="H223" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I223" t="s">
         <v>11</v>
@@ -6912,10 +6912,10 @@
         <v>12</v>
       </c>
       <c r="D224" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E224" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F224" t="s">
         <v>11</v>
@@ -6924,7 +6924,7 @@
         <v>12</v>
       </c>
       <c r="H224" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I224" t="s">
         <v>11</v>
@@ -6938,7 +6938,7 @@
         <v>11</v>
       </c>
       <c r="C225" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -6953,7 +6953,7 @@
         <v>12</v>
       </c>
       <c r="H225" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I225" t="s">
         <v>11</v>
@@ -6973,7 +6973,7 @@
         <v>11</v>
       </c>
       <c r="E226" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F226" t="s">
         <v>11</v>
@@ -6982,7 +6982,7 @@
         <v>12</v>
       </c>
       <c r="H226" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I226" t="s">
         <v>11</v>
@@ -6996,22 +6996,22 @@
         <v>11</v>
       </c>
       <c r="C227" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D227" t="s">
         <v>11</v>
       </c>
       <c r="E227" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F227" t="s">
         <v>11</v>
       </c>
       <c r="G227" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H227" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I227" t="s">
         <v>11</v>
@@ -7022,22 +7022,22 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C228" t="s">
         <v>12</v>
       </c>
       <c r="D228" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E228" t="s">
         <v>13</v>
       </c>
       <c r="F228" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G228" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H228" t="s">
         <v>12</v>
@@ -7057,7 +7057,7 @@
         <v>12</v>
       </c>
       <c r="D229" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E229" t="s">
         <v>12</v>
@@ -7086,10 +7086,10 @@
         <v>12</v>
       </c>
       <c r="D230" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E230" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F230" t="s">
         <v>11</v>
@@ -7098,7 +7098,7 @@
         <v>12</v>
       </c>
       <c r="H230" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I230" t="s">
         <v>11</v>
@@ -7118,7 +7118,7 @@
         <v>11</v>
       </c>
       <c r="E231" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F231" t="s">
         <v>11</v>
@@ -7127,7 +7127,7 @@
         <v>12</v>
       </c>
       <c r="H231" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I231" t="s">
         <v>11</v>
@@ -7144,10 +7144,10 @@
         <v>12</v>
       </c>
       <c r="D232" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E232" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F232" t="s">
         <v>11</v>
@@ -7176,13 +7176,13 @@
         <v>11</v>
       </c>
       <c r="E233" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F233" t="s">
         <v>11</v>
       </c>
       <c r="G233" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H233" t="s">
         <v>12</v>
@@ -7205,7 +7205,7 @@
         <v>11</v>
       </c>
       <c r="E234" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F234" t="s">
         <v>11</v>
@@ -7214,7 +7214,7 @@
         <v>12</v>
       </c>
       <c r="H234" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I234" t="s">
         <v>11</v>
@@ -7243,7 +7243,7 @@
         <v>11</v>
       </c>
       <c r="H235" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I235" t="s">
         <v>11</v>
@@ -7260,10 +7260,10 @@
         <v>12</v>
       </c>
       <c r="D236" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E236" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F236" t="s">
         <v>11</v>
@@ -7272,7 +7272,7 @@
         <v>12</v>
       </c>
       <c r="H236" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I236" t="s">
         <v>11</v>
@@ -7289,19 +7289,19 @@
         <v>12</v>
       </c>
       <c r="D237" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E237" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F237" t="s">
         <v>11</v>
       </c>
       <c r="G237" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H237" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I237" t="s">
         <v>11</v>
@@ -7318,10 +7318,10 @@
         <v>12</v>
       </c>
       <c r="D238" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E238" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F238" t="s">
         <v>11</v>
@@ -7330,7 +7330,7 @@
         <v>12</v>
       </c>
       <c r="H238" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I238" t="s">
         <v>12</v>
@@ -7388,7 +7388,7 @@
         <v>12</v>
       </c>
       <c r="H240" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I240" t="s">
         <v>11</v>
@@ -7405,10 +7405,10 @@
         <v>12</v>
       </c>
       <c r="D241" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E241" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F241" t="s">
         <v>11</v>
@@ -7417,10 +7417,10 @@
         <v>12</v>
       </c>
       <c r="H241" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I241" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -7431,13 +7431,13 @@
         <v>11</v>
       </c>
       <c r="C242" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D242" t="s">
         <v>11</v>
       </c>
       <c r="E242" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F242" t="s">
         <v>11</v>
@@ -7446,7 +7446,7 @@
         <v>12</v>
       </c>
       <c r="H242" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I242" t="s">
         <v>11</v>
@@ -7460,13 +7460,13 @@
         <v>11</v>
       </c>
       <c r="C243" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D243" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E243" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F243" t="s">
         <v>11</v>
@@ -7475,7 +7475,7 @@
         <v>12</v>
       </c>
       <c r="H243" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I243" t="s">
         <v>11</v>
@@ -7489,22 +7489,22 @@
         <v>11</v>
       </c>
       <c r="C244" t="s">
+        <v>14</v>
+      </c>
+      <c r="D244" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244" t="s">
         <v>15</v>
       </c>
-      <c r="D244" t="s">
-        <v>11</v>
-      </c>
-      <c r="E244" t="s">
-        <v>16</v>
-      </c>
       <c r="F244" t="s">
         <v>12</v>
       </c>
       <c r="G244" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H244" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I244" t="s">
         <v>12</v>
@@ -7518,13 +7518,13 @@
         <v>11</v>
       </c>
       <c r="C245" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D245" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E245" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F245" t="s">
         <v>12</v>
@@ -7533,7 +7533,7 @@
         <v>12</v>
       </c>
       <c r="H245" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I245" t="s">
         <v>11</v>
@@ -7550,10 +7550,10 @@
         <v>12</v>
       </c>
       <c r="D246" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E246" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F246" t="s">
         <v>11</v>
@@ -7562,7 +7562,7 @@
         <v>12</v>
       </c>
       <c r="H246" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I246" t="s">
         <v>11</v>
@@ -7591,7 +7591,7 @@
         <v>12</v>
       </c>
       <c r="H247" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I247" t="s">
         <v>11</v>
@@ -7649,7 +7649,7 @@
         <v>12</v>
       </c>
       <c r="H249" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I249" t="s">
         <v>11</v>
@@ -7669,7 +7669,7 @@
         <v>11</v>
       </c>
       <c r="E250" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F250" t="s">
         <v>11</v>
@@ -7698,7 +7698,7 @@
         <v>11</v>
       </c>
       <c r="E251" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F251" t="s">
         <v>11</v>
@@ -7727,7 +7727,7 @@
         <v>11</v>
       </c>
       <c r="E252" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F252" t="s">
         <v>11</v>
@@ -7739,7 +7739,7 @@
         <v>12</v>
       </c>
       <c r="I252" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="253" spans="1:9">
@@ -7756,7 +7756,7 @@
         <v>11</v>
       </c>
       <c r="E253" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F253" t="s">
         <v>11</v>
@@ -7765,7 +7765,7 @@
         <v>12</v>
       </c>
       <c r="H253" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I253" t="s">
         <v>11</v>
@@ -7785,7 +7785,7 @@
         <v>11</v>
       </c>
       <c r="E254" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F254" t="s">
         <v>11</v>
@@ -7794,7 +7794,7 @@
         <v>12</v>
       </c>
       <c r="H254" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I254" t="s">
         <v>11</v>
@@ -7814,7 +7814,7 @@
         <v>12</v>
       </c>
       <c r="E255" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F255" t="s">
         <v>11</v>
@@ -7823,7 +7823,7 @@
         <v>12</v>
       </c>
       <c r="H255" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I255" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
reemplazar 0 en el marco por 1a
</commit_message>
<xml_diff>
--- a/data/Marco acumulativo.xlsx
+++ b/data/Marco acumulativo.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\DSProjects\CFK2022\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29576E15-75E9-48F0-A5C0-A94DD3B95B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$255</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="18">
   <si>
     <t>Código IE</t>
   </si>
@@ -64,9 +73,6 @@
     <t>2B</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -76,8 +82,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +146,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +232,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +284,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,14 +477,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I255"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72:E237"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -492,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -550,7 +602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -579,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -605,10 +657,10 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -637,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -666,7 +718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -695,7 +747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -724,7 +776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -750,10 +802,10 @@
         <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -782,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -811,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -837,10 +889,10 @@
         <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -869,7 +921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -898,7 +950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -927,7 +979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -956,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -985,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1014,7 +1066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1043,7 +1095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1072,7 +1124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1101,7 +1153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1130,7 +1182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1159,7 +1211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1188,7 +1240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1217,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1246,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1275,7 +1327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1304,7 +1356,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1333,7 +1385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1362,7 +1414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1391,7 +1443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1420,7 +1472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1449,7 +1501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1478,7 +1530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1507,7 +1559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1536,7 +1588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1565,7 +1617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1594,7 +1646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1623,7 +1675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1652,7 +1704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1681,7 +1733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1710,7 +1762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1739,7 +1791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1768,7 +1820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1797,7 +1849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1826,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1855,7 +1907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1884,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1913,7 +1965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1942,7 +1994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1968,10 +2020,10 @@
         <v>12</v>
       </c>
       <c r="I53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2000,7 +2052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2029,7 +2081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2058,7 +2110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2087,7 +2139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2116,7 +2168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2145,7 +2197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2174,7 +2226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2203,7 +2255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2232,7 +2284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2261,7 +2313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2290,7 +2342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2319,7 +2371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2348,7 +2400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2377,7 +2429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2406,7 +2458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2435,7 +2487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2464,7 +2516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2493,7 +2545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2504,10 +2556,10 @@
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F72" t="s">
         <v>11</v>
@@ -2522,7 +2574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2551,7 +2603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2580,7 +2632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2609,7 +2661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2638,7 +2690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2667,7 +2719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2696,7 +2748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2725,7 +2777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2783,7 +2835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2812,7 +2864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2841,7 +2893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2852,10 +2904,10 @@
         <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E84" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F84" t="s">
         <v>11</v>
@@ -2870,7 +2922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2899,7 +2951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2928,7 +2980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2957,7 +3009,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2986,7 +3038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3015,7 +3067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3044,7 +3096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3073,7 +3125,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3090,19 +3142,19 @@
         <v>12</v>
       </c>
       <c r="F92" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" t="s">
         <v>17</v>
       </c>
-      <c r="G92" t="s">
-        <v>17</v>
-      </c>
-      <c r="H92" t="s">
-        <v>12</v>
-      </c>
-      <c r="I92" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3131,7 +3183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3160,7 +3212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3189,7 +3241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3218,7 +3270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3247,7 +3299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3276,7 +3328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3305,7 +3357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3334,7 +3386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3363,7 +3415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3374,10 +3426,10 @@
         <v>12</v>
       </c>
       <c r="D102" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E102" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F102" t="s">
         <v>11</v>
@@ -3392,7 +3444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3421,7 +3473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3450,7 +3502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3479,7 +3531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3508,7 +3560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3537,7 +3589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3566,7 +3618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3595,7 +3647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3624,7 +3676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3653,7 +3705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3682,7 +3734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3711,7 +3763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3740,7 +3792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3769,7 +3821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3798,7 +3850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3827,7 +3879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3856,7 +3908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3885,7 +3937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3914,7 +3966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3943,7 +3995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3972,7 +4024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4001,7 +4053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4030,7 +4082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4059,7 +4111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4088,7 +4140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4117,7 +4169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4146,7 +4198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4175,7 +4227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4204,7 +4256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4233,7 +4285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4262,7 +4314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4291,7 +4343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4320,7 +4372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4349,7 +4401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4378,7 +4430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4407,7 +4459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4436,7 +4488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4465,7 +4517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4494,7 +4546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4523,7 +4575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4534,10 +4586,10 @@
         <v>12</v>
       </c>
       <c r="D142" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E142" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F142" t="s">
         <v>11</v>
@@ -4552,7 +4604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4581,7 +4633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4610,7 +4662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4639,7 +4691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4668,7 +4720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4679,10 +4731,10 @@
         <v>12</v>
       </c>
       <c r="D147" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E147" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F147" t="s">
         <v>11</v>
@@ -4697,7 +4749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4726,7 +4778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4746,7 +4798,7 @@
         <v>13</v>
       </c>
       <c r="G149" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H149" t="s">
         <v>12</v>
@@ -4755,7 +4807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4784,7 +4836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4813,7 +4865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4842,7 +4894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4871,7 +4923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4900,7 +4952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4929,7 +4981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4958,7 +5010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4987,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5016,7 +5068,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5045,7 +5097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5074,7 +5126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5103,7 +5155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5132,7 +5184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5161,7 +5213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5190,7 +5242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5219,7 +5271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5248,7 +5300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5277,7 +5329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5306,7 +5358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5335,7 +5387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5364,7 +5416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5393,7 +5445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5422,7 +5474,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5451,7 +5503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5480,7 +5532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5509,7 +5561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5538,7 +5590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5567,7 +5619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5596,7 +5648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5625,7 +5677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5654,7 +5706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5683,7 +5735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5712,7 +5764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5741,7 +5793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5770,7 +5822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5799,7 +5851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5828,7 +5880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5857,7 +5909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5886,7 +5938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5915,7 +5967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5944,7 +5996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5973,7 +6025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6002,7 +6054,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6031,7 +6083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6060,7 +6112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6089,7 +6141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6118,7 +6170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6147,7 +6199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6176,7 +6228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6205,7 +6257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6234,7 +6286,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6263,7 +6315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6274,10 +6326,10 @@
         <v>12</v>
       </c>
       <c r="D202" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E202" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F202" t="s">
         <v>11</v>
@@ -6292,7 +6344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6321,7 +6373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6350,7 +6402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6379,7 +6431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6408,7 +6460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6437,7 +6489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6466,7 +6518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6495,7 +6547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6524,7 +6576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6553,7 +6605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>211</v>
       </c>
@@ -6582,7 +6634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6611,7 +6663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6640,7 +6692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6669,7 +6721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>215</v>
       </c>
@@ -6698,7 +6750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6727,7 +6779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6756,7 +6808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6785,7 +6837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>219</v>
       </c>
@@ -6814,7 +6866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>220</v>
       </c>
@@ -6843,7 +6895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>221</v>
       </c>
@@ -6872,7 +6924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>222</v>
       </c>
@@ -6901,7 +6953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6930,7 +6982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>224</v>
       </c>
@@ -6959,7 +7011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>225</v>
       </c>
@@ -6988,7 +7040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>226</v>
       </c>
@@ -7017,7 +7069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>227</v>
       </c>
@@ -7046,7 +7098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>228</v>
       </c>
@@ -7075,7 +7127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>229</v>
       </c>
@@ -7104,7 +7156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>230</v>
       </c>
@@ -7133,7 +7185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>231</v>
       </c>
@@ -7162,7 +7214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>232</v>
       </c>
@@ -7191,7 +7243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>233</v>
       </c>
@@ -7220,7 +7272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>234</v>
       </c>
@@ -7249,7 +7301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>235</v>
       </c>
@@ -7278,7 +7330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>236</v>
       </c>
@@ -7289,10 +7341,10 @@
         <v>12</v>
       </c>
       <c r="D237" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E237" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F237" t="s">
         <v>11</v>
@@ -7307,7 +7359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>237</v>
       </c>
@@ -7336,7 +7388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>238</v>
       </c>
@@ -7365,7 +7417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>239</v>
       </c>
@@ -7394,7 +7446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>240</v>
       </c>
@@ -7423,7 +7475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>241</v>
       </c>
@@ -7452,7 +7504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>242</v>
       </c>
@@ -7481,7 +7533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>243</v>
       </c>
@@ -7510,7 +7562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>244</v>
       </c>
@@ -7539,7 +7591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>245</v>
       </c>
@@ -7568,7 +7620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>246</v>
       </c>
@@ -7597,7 +7649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>247</v>
       </c>
@@ -7626,7 +7678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>248</v>
       </c>
@@ -7655,7 +7707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>249</v>
       </c>
@@ -7684,7 +7736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>250</v>
       </c>
@@ -7713,7 +7765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>251</v>
       </c>
@@ -7742,7 +7794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>252</v>
       </c>
@@ -7771,7 +7823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>9</v>
       </c>
@@ -7800,7 +7852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>10</v>
       </c>
@@ -7830,6 +7882,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I255" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>